<commit_message>
Added code for selenium grid setup
</commit_message>
<xml_diff>
--- a/DataDrivenFile.xlsx
+++ b/DataDrivenFile.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8B2CA21E-5DB8-4517-A99E-2F32CC4F9F08}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{3644E4B4-8D22-4763-ADED-F156FBAB4C4E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1520" yWindow="1520" windowWidth="19460" windowHeight="11060" xr2:uid="{958CC76F-C632-4C73-9EC4-A914EC67275E}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>ID</t>
   </si>
@@ -29,10 +29,16 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>sumitIdentity1</t>
-  </si>
-  <si>
-    <t>SummitPass1</t>
+    <t>sumitIdentity7</t>
+  </si>
+  <si>
+    <t>SummitPass7</t>
+  </si>
+  <si>
+    <t>sumitIdentity8</t>
+  </si>
+  <si>
+    <t>SummitPass8</t>
   </si>
 </sst>
 </file>
@@ -387,7 +393,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -408,7 +414,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35"/>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35"/>

</xml_diff>